<commit_message>
Aktualisiere E-Mail-Inhalt mit Kursangebot und füge neue Teilnehmerinformationen hinzu; aktualisiere die mails.xlsx Datei.
</commit_message>
<xml_diff>
--- a/mails.xlsx
+++ b/mails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Spammer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B29BBB21-7F99-4B35-A798-412EC5B1DAB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3F601F0-AE78-4C94-AE7D-B01205075C1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1950" yWindow="1950" windowWidth="28800" windowHeight="15645" xr2:uid="{37D975CF-16CE-46BF-9EE8-8A1F497DE61C}"/>
   </bookViews>
@@ -36,9 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>jtuttas@gmx.net</t>
+  </si>
+  <si>
+    <t>kelker@kelker.de</t>
   </si>
 </sst>
 </file>
@@ -421,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACBFB63B-EF68-4515-9EE3-00B9A42AFCC1}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -437,11 +440,17 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" xr:uid="{97172FA8-5D4D-4F93-ADF7-08014D846E5E}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{1884E301-7F80-407E-9A80-C2EF3AF6A537}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>